<commit_message>
changes to the code to explore the efficiency limit
added the possilbility to run the limit of efficiency based on the parameters of the EES paper, and added some scripts
</commit_message>
<xml_diff>
--- a/parameters/DeviceParameters_Default.xlsx
+++ b/parameters/DeviceParameters_Default.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ma11115\Box\Github_mohammed_azzouzi\DriftFusion_OPV\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ma11115\Box\github_folder\DriftFusionOPV\parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D7984D9-E01A-4B43-BDAA-9E23FA2BDD1B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A994A08-6C85-4E6D-B1FF-157AE9394492}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -469,8 +469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="X6" sqref="X6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -483,6 +483,12 @@
     <col min="10" max="10" width="24.6640625" customWidth="1"/>
     <col min="17" max="17" width="37.21875" customWidth="1"/>
     <col min="18" max="18" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="33.33203125" customWidth="1"/>
+    <col min="31" max="31" width="25.109375" customWidth="1"/>
+    <col min="32" max="32" width="28.77734375" customWidth="1"/>
+    <col min="33" max="33" width="30.33203125" customWidth="1"/>
+    <col min="34" max="34" width="30" customWidth="1"/>
+    <col min="35" max="35" width="31.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.3">
@@ -710,22 +716,22 @@
         <v>0</v>
       </c>
       <c r="AD3" s="1">
-        <v>1000000000000</v>
+        <v>1</v>
       </c>
       <c r="AE3" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AF3" s="1">
-        <v>1E-10</v>
+        <v>1.0000000000000001E-15</v>
       </c>
       <c r="AG3" s="1">
-        <v>3000000000000</v>
+        <v>1</v>
       </c>
       <c r="AH3" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AI3" s="1">
-        <v>3000000000000</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.3">
@@ -912,22 +918,22 @@
         <v>0</v>
       </c>
       <c r="AD5" s="1">
-        <v>1000000000000</v>
+        <v>1</v>
       </c>
       <c r="AE5" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AF5" s="1">
-        <v>1E-10</v>
+        <v>1.0000000000000001E-15</v>
       </c>
       <c r="AG5" s="1">
-        <v>3000000000000</v>
+        <v>1</v>
       </c>
       <c r="AH5" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AI5" s="1">
-        <v>3000000000000</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.3">

</xml_diff>